<commit_message>
Just for recording to record current situation.
</commit_message>
<xml_diff>
--- a/blanco-meta/telegramsKt/HttpCommonRequest.xlsx
+++ b/blanco-meta/telegramsKt/HttpCommonRequest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/cacco/oplux/oplux-meta/meta/telegramsKt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/telegramsKt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69271C8F-8CB0-8C41-B8DE-B848B4D55B92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881C12BE-9109-2C4C-B414-EB5856829E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
   <si>
     <t>クラス名</t>
   </si>
@@ -588,6 +588,28 @@
     </rPh>
     <rPh sb="17" eb="19">
       <t xml:space="preserve">フヨウナ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>rawBody</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>生のbodyデータを格納します。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ナマノ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">カクノウ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1539,24 +1561,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1568,24 +1589,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1598,7 +1618,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1614,7 +1634,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1680,19 +1700,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="52" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1706,7 +1717,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1726,16 +1737,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="53" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1763,7 +1774,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1787,7 +1798,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2203,18 +2214,18 @@
   </sheetPr>
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+    <sheetView tabSelected="1" topLeftCell="F12" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
-    <col min="7" max="10" width="20.1640625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="10" style="31" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="31" customWidth="1"/>
-    <col min="13" max="13" width="9.5" style="31" customWidth="1"/>
+    <col min="7" max="10" width="20.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="1" customWidth="1"/>
     <col min="14" max="18" width="9" style="1" customWidth="1"/>
     <col min="19" max="19" width="13.1640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="6.83203125" style="1" customWidth="1"/>
@@ -2249,15 +2260,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="82"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="76"/>
-      <c r="U5" s="76"/>
+      <c r="F5" s="75"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="3" t="s">
@@ -2269,15 +2272,7 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="83"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="76"/>
+      <c r="F6" s="76"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="3" t="s">
@@ -2287,17 +2282,9 @@
       <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="84"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="76"/>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="3" t="s">
@@ -2307,73 +2294,49 @@
       <c r="C8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="31" t="s">
+      <c r="F8" s="70"/>
+      <c r="G8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-    </row>
-    <row r="9" spans="1:21" s="31" customFormat="1">
-      <c r="A9" s="52" t="s">
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="70" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="71"/>
+      <c r="D9" s="69"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="84"/>
-    </row>
-    <row r="10" spans="1:21" s="31" customFormat="1">
-      <c r="A10" s="107" t="s">
+      <c r="F9" s="70"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="70" t="s">
+      <c r="B10" s="99"/>
+      <c r="C10" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="72"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="77"/>
-      <c r="R10" s="77"/>
-      <c r="S10" s="77"/>
-      <c r="T10" s="77"/>
-      <c r="U10" s="77"/>
-    </row>
-    <row r="11" spans="1:21" s="31" customFormat="1">
-      <c r="A11" s="52" t="s">
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="97" t="s">
+      <c r="B11" s="51"/>
+      <c r="C11" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="85"/>
-      <c r="M11" s="95"/>
-      <c r="N11" s="77"/>
-      <c r="O11" s="77"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="77"/>
-      <c r="R11" s="77"/>
-      <c r="S11" s="77"/>
-      <c r="T11" s="77"/>
-      <c r="U11" s="77"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="76"/>
+      <c r="M11" s="86"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
@@ -2385,15 +2348,7 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="83"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="76"/>
-      <c r="S12" s="76"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="76"/>
+      <c r="F12" s="76"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="3" t="s">
@@ -2405,23 +2360,15 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="83"/>
+      <c r="F13" s="76"/>
       <c r="M13"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
-      <c r="S13" s="76"/>
-      <c r="T13" s="76"/>
-      <c r="U13" s="76"/>
-    </row>
-    <row r="14" spans="1:21" s="31" customFormat="1">
-      <c r="A14" s="49" t="s">
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
@@ -2435,12 +2382,12 @@
       <c r="N14"/>
       <c r="O14"/>
     </row>
-    <row r="15" spans="1:21" s="31" customFormat="1">
-      <c r="A15" s="49" t="s">
+    <row r="15" spans="1:21">
+      <c r="A15" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="51" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="49" t="s">
         <v>38</v>
       </c>
       <c r="D15" t="s">
@@ -2458,12 +2405,12 @@
       <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:21" s="31" customFormat="1">
-      <c r="A16" s="49" t="s">
+    <row r="16" spans="1:21">
+      <c r="A16" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
@@ -2477,12 +2424,12 @@
       <c r="N16"/>
       <c r="O16"/>
     </row>
-    <row r="17" spans="1:21" s="31" customFormat="1">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:20">
+      <c r="A17" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="49" t="s">
         <v>38</v>
       </c>
       <c r="D17"/>
@@ -2498,12 +2445,12 @@
       <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:21" s="31" customFormat="1">
-      <c r="A18" s="49" t="s">
+    <row r="18" spans="1:20">
+      <c r="A18" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -2514,21 +2461,14 @@
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="78"/>
-      <c r="O18" s="77"/>
-      <c r="P18" s="77"/>
-      <c r="Q18" s="77"/>
-      <c r="R18" s="77"/>
-      <c r="S18" s="77"/>
-      <c r="T18" s="77"/>
-      <c r="U18" s="77"/>
-    </row>
-    <row r="19" spans="1:21" s="31" customFormat="1">
-      <c r="A19" s="49" t="s">
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="49" t="s">
         <v>38</v>
       </c>
       <c r="D19"/>
@@ -2540,21 +2480,14 @@
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
-      <c r="N19" s="78"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77"/>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="77"/>
-      <c r="S19" s="77"/>
-      <c r="T19" s="77"/>
-      <c r="U19" s="77"/>
-    </row>
-    <row r="20" spans="1:21" s="31" customFormat="1">
-      <c r="A20" s="49" t="s">
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -2564,21 +2497,14 @@
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
-      <c r="N20" s="78"/>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="77"/>
-      <c r="S20" s="77"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="77"/>
-    </row>
-    <row r="21" spans="1:21" s="31" customFormat="1">
-      <c r="A21" s="68" t="s">
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="69"/>
-      <c r="C21" s="51" t="s">
+      <c r="B21" s="67"/>
+      <c r="C21" s="49" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
@@ -2591,130 +2517,95 @@
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="78"/>
-      <c r="O21" s="78"/>
-      <c r="P21" s="78"/>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="78"/>
-      <c r="S21" s="78"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="77"/>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="M21" s="71"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
-      <c r="N22" s="79"/>
-      <c r="O22" s="79"/>
-      <c r="P22" s="79"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="79"/>
-      <c r="S22" s="79"/>
-      <c r="T22" s="79"/>
-      <c r="U22" s="76"/>
-    </row>
-    <row r="23" spans="1:21" s="31" customFormat="1">
-      <c r="A23" s="28" t="s">
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="77"/>
-      <c r="U23" s="77"/>
-    </row>
-    <row r="24" spans="1:21" s="31" customFormat="1">
-      <c r="A24" s="32" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="77"/>
-      <c r="S24" s="77"/>
-      <c r="T24" s="77"/>
-      <c r="U24" s="77"/>
-    </row>
-    <row r="25" spans="1:21" s="31" customFormat="1">
-      <c r="A25" s="52" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="77"/>
-      <c r="T25" s="77"/>
-      <c r="U25" s="77"/>
-    </row>
-    <row r="26" spans="1:21" s="31" customFormat="1">
-      <c r="A26" s="52" t="s">
+      <c r="B25" s="51"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="77"/>
-      <c r="T26" s="77"/>
-      <c r="U26" s="77"/>
-    </row>
-    <row r="27" spans="1:21" s="31" customFormat="1">
+      <c r="B26" s="51"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -2727,237 +2618,157 @@
       <c r="J27"/>
       <c r="K27"/>
       <c r="L27"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="78"/>
-      <c r="O27" s="77"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="77"/>
-      <c r="R27" s="77"/>
-      <c r="S27" s="77"/>
-      <c r="T27" s="77"/>
-      <c r="U27" s="77"/>
-    </row>
-    <row r="28" spans="1:21" s="31" customFormat="1">
+      <c r="M27" s="72"/>
+      <c r="N27"/>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="77"/>
-      <c r="N28" s="77"/>
-      <c r="O28" s="77"/>
-      <c r="P28" s="77"/>
-      <c r="Q28" s="77"/>
-      <c r="R28" s="77"/>
-      <c r="S28" s="77"/>
-      <c r="T28" s="77"/>
-      <c r="U28" s="77"/>
-    </row>
-    <row r="29" spans="1:21" s="31" customFormat="1">
-      <c r="A29" s="114" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="89"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="114" t="s">
+      <c r="B29" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="113" t="s">
+      <c r="C29" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="113" t="s">
+      <c r="D29" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="121" t="s">
+      <c r="E29" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="80"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="77"/>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="77"/>
-      <c r="R29" s="77"/>
-      <c r="S29" s="77"/>
-      <c r="T29" s="77"/>
-      <c r="U29" s="77"/>
-    </row>
-    <row r="30" spans="1:21" s="31" customFormat="1">
-      <c r="A30" s="114"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="113"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="77"/>
-      <c r="T30" s="77"/>
-      <c r="U30" s="77"/>
-    </row>
-    <row r="31" spans="1:21" s="31" customFormat="1">
-      <c r="A31" s="16">
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="105"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="104"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="15">
         <v>1</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="99" t="s">
+      <c r="E31" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="80"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="73"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="77"/>
-      <c r="R31" s="77"/>
-      <c r="S31" s="77"/>
-      <c r="T31" s="77"/>
-      <c r="U31" s="77"/>
-    </row>
-    <row r="32" spans="1:21" s="31" customFormat="1">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="77"/>
-      <c r="R32" s="77"/>
-      <c r="S32" s="77"/>
-      <c r="T32" s="77"/>
-      <c r="U32" s="77"/>
-    </row>
-    <row r="33" spans="1:23" s="31" customFormat="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="73"/>
-      <c r="M33" s="73"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
-      <c r="R33" s="77"/>
-      <c r="S33" s="77"/>
-      <c r="T33" s="77"/>
-      <c r="U33" s="77"/>
-    </row>
-    <row r="34" spans="1:23" s="31" customFormat="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="77"/>
-      <c r="R34" s="77"/>
-      <c r="S34" s="77"/>
-      <c r="T34" s="77"/>
-      <c r="U34" s="77"/>
-    </row>
-    <row r="35" spans="1:23" s="31" customFormat="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-      <c r="N35" s="77"/>
-      <c r="O35" s="77"/>
-      <c r="P35" s="77"/>
-      <c r="Q35" s="77"/>
-      <c r="R35" s="77"/>
-      <c r="S35" s="77"/>
-      <c r="T35" s="77"/>
-      <c r="U35" s="77"/>
-    </row>
-    <row r="36" spans="1:23" s="31" customFormat="1">
-      <c r="A36" s="100"/>
-      <c r="B36" s="101"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="77"/>
-      <c r="O36" s="77"/>
-      <c r="P36" s="77"/>
-      <c r="Q36" s="77"/>
-      <c r="R36" s="77"/>
-      <c r="S36" s="77"/>
-      <c r="T36" s="77"/>
-      <c r="U36" s="77"/>
-    </row>
-    <row r="37" spans="1:23" s="31" customFormat="1">
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="15"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33" s="15"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" s="15"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36" s="91"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="71"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="71"/>
+    </row>
+    <row r="37" spans="1:23">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -2970,164 +2781,124 @@
       <c r="J37"/>
       <c r="K37"/>
       <c r="L37"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="78"/>
-      <c r="O37" s="77"/>
-      <c r="P37" s="77"/>
-      <c r="Q37" s="77"/>
-      <c r="R37" s="77"/>
-      <c r="S37" s="77"/>
-      <c r="T37" s="77"/>
-      <c r="U37" s="77"/>
-    </row>
-    <row r="38" spans="1:23" s="31" customFormat="1">
-      <c r="A38" s="28" t="s">
+      <c r="M37" s="72"/>
+      <c r="N37"/>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
-      <c r="R38" s="77"/>
-      <c r="S38" s="77"/>
-      <c r="T38" s="77"/>
-      <c r="U38" s="77"/>
-    </row>
-    <row r="39" spans="1:23" s="31" customFormat="1">
-      <c r="A39" s="56" t="s">
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="M38" s="72"/>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="57" t="s">
+      <c r="B39" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="73"/>
-      <c r="M39" s="74"/>
-      <c r="N39" s="80"/>
-      <c r="O39" s="77"/>
-      <c r="P39" s="81"/>
-      <c r="Q39" s="81"/>
-      <c r="R39" s="77"/>
-      <c r="S39" s="77"/>
-      <c r="T39" s="77"/>
-      <c r="U39" s="77"/>
-    </row>
-    <row r="40" spans="1:23" s="31" customFormat="1">
-      <c r="A40" s="58">
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="71"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="71"/>
+      <c r="P39" s="74"/>
+      <c r="Q39" s="74"/>
+    </row>
+    <row r="40" spans="1:23">
+      <c r="A40" s="56">
         <v>1</v>
       </c>
-      <c r="B40" s="59" t="s">
+      <c r="B40" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="74"/>
-      <c r="L40" s="74"/>
-      <c r="N40" s="77"/>
-      <c r="O40" s="78"/>
-      <c r="P40" s="78"/>
-      <c r="Q40" s="78"/>
-      <c r="R40" s="77"/>
-      <c r="S40" s="77"/>
-      <c r="T40" s="77"/>
-      <c r="U40" s="77"/>
-    </row>
-    <row r="41" spans="1:23" s="31" customFormat="1">
-      <c r="A41" s="58">
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+    </row>
+    <row r="41" spans="1:23">
+      <c r="A41" s="56">
         <v>2</v>
       </c>
-      <c r="B41" s="59" t="s">
+      <c r="B41" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="74"/>
-      <c r="N41" s="77"/>
-      <c r="O41" s="78"/>
-      <c r="P41" s="78"/>
-      <c r="Q41" s="78"/>
-      <c r="R41" s="77"/>
-      <c r="S41" s="77"/>
-      <c r="T41" s="77"/>
-      <c r="U41" s="77"/>
-    </row>
-    <row r="42" spans="1:23" s="31" customFormat="1">
-      <c r="A42" s="58">
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
+      <c r="K41" s="72"/>
+      <c r="L41" s="72"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="A42" s="56">
         <v>3</v>
       </c>
-      <c r="B42" s="59" t="s">
+      <c r="B42" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="74"/>
-      <c r="N42" s="77"/>
-      <c r="O42" s="78"/>
-      <c r="P42" s="78"/>
-      <c r="Q42" s="78"/>
-      <c r="R42" s="77"/>
-      <c r="S42" s="77"/>
-      <c r="T42" s="77"/>
-      <c r="U42" s="77"/>
-    </row>
-    <row r="43" spans="1:23" s="31" customFormat="1">
-      <c r="A43" s="64"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="74"/>
-      <c r="L43" s="74"/>
-      <c r="M43" s="73"/>
-      <c r="N43" s="77"/>
-      <c r="O43" s="78"/>
-      <c r="P43" s="78"/>
-      <c r="Q43" s="78"/>
-      <c r="R43" s="77"/>
-      <c r="S43" s="77"/>
-      <c r="T43" s="77"/>
-      <c r="U43" s="77"/>
-    </row>
-    <row r="44" spans="1:23" s="31" customFormat="1">
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+    </row>
+    <row r="43" spans="1:23">
+      <c r="A43" s="62"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="71"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+    </row>
+    <row r="44" spans="1:23">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -3140,7 +2911,7 @@
       <c r="J44"/>
       <c r="K44"/>
       <c r="L44"/>
-      <c r="M44" s="74"/>
+      <c r="M44" s="72"/>
       <c r="N44"/>
       <c r="O44"/>
     </row>
@@ -3148,632 +2919,645 @@
       <c r="A45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
       <c r="V45" s="5"/>
-      <c r="W45" s="12"/>
+      <c r="W45" s="11"/>
     </row>
     <row r="46" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="114" t="s">
+      <c r="B46" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="113" t="s">
+      <c r="C46" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="113" t="s">
+      <c r="D46" s="104" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="115" t="s">
+      <c r="E46" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="113" t="s">
+      <c r="F46" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="113" t="s">
+      <c r="G46" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="H46" s="113" t="s">
+      <c r="H46" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="I46" s="113" t="s">
+      <c r="I46" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="J46" s="117" t="s">
+      <c r="J46" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="K46" s="117" t="s">
+      <c r="K46" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="L46" s="109" t="s">
+      <c r="L46" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="M46" s="119" t="s">
+      <c r="M46" s="110" t="s">
         <v>63</v>
       </c>
-      <c r="N46" s="111" t="s">
+      <c r="N46" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="O46" s="112"/>
-      <c r="P46" s="111" t="s">
+      <c r="O46" s="103"/>
+      <c r="P46" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="Q46" s="112"/>
-      <c r="R46" s="37" t="s">
+      <c r="Q46" s="103"/>
+      <c r="R46" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S46" s="113" t="s">
+      <c r="S46" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="T46" s="113"/>
-      <c r="U46" s="13"/>
-      <c r="V46" s="14"/>
+      <c r="T46" s="104"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="13"/>
       <c r="W46" s="7"/>
     </row>
     <row r="47" spans="1:23">
-      <c r="A47" s="114"/>
-      <c r="B47" s="114"/>
-      <c r="C47" s="113"/>
-      <c r="D47" s="113"/>
-      <c r="E47" s="116"/>
-      <c r="F47" s="113"/>
-      <c r="G47" s="113"/>
-      <c r="H47" s="113"/>
-      <c r="I47" s="113"/>
-      <c r="J47" s="118"/>
-      <c r="K47" s="118"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="120"/>
-      <c r="N47" s="38" t="s">
+      <c r="A47" s="105"/>
+      <c r="B47" s="105"/>
+      <c r="C47" s="104"/>
+      <c r="D47" s="104"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="104"/>
+      <c r="I47" s="104"/>
+      <c r="J47" s="109"/>
+      <c r="K47" s="109"/>
+      <c r="L47" s="101"/>
+      <c r="M47" s="111"/>
+      <c r="N47" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="O47" s="38" t="s">
+      <c r="O47" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="P47" s="38" t="s">
+      <c r="P47" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="Q47" s="38" t="s">
+      <c r="Q47" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="R47" s="38" t="s">
+      <c r="R47" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="S47" s="113"/>
-      <c r="T47" s="113"/>
-      <c r="U47" s="15"/>
-      <c r="V47" s="27"/>
-      <c r="W47" s="12"/>
+      <c r="S47" s="104"/>
+      <c r="T47" s="104"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="11"/>
     </row>
     <row r="48" spans="1:23" ht="30">
-      <c r="A48" s="16">
+      <c r="A48" s="15">
         <v>1</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="H48" s="90" t="s">
+      <c r="H48" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="I48" s="104" t="s">
+      <c r="I48" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="J48" s="90"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="86" t="s">
+      <c r="J48" s="81"/>
+      <c r="K48" s="97"/>
+      <c r="L48" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="M48" s="87" t="s">
+      <c r="M48" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="N48" s="39"/>
-      <c r="O48" s="40"/>
-      <c r="P48" s="39"/>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="41"/>
-      <c r="S48" s="18" t="s">
+      <c r="N48" s="37"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="39"/>
+      <c r="S48" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="26"/>
-      <c r="W48" s="12"/>
+      <c r="T48" s="18"/>
+      <c r="U48" s="18"/>
+      <c r="V48" s="25"/>
+      <c r="W48" s="11"/>
     </row>
     <row r="49" spans="1:23">
-      <c r="A49" s="16">
+      <c r="A49" s="15">
         <f>A48+1</f>
         <v>2</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="105"/>
-      <c r="J49" s="18" t="b">
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="96"/>
+      <c r="J49" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="K49" s="87"/>
-      <c r="L49" s="87" t="s">
+      <c r="K49" s="78"/>
+      <c r="L49" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="M49" s="87" t="s">
+      <c r="M49" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18" t="s">
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="T49" s="19"/>
-      <c r="U49" s="19"/>
-      <c r="V49" s="20"/>
-      <c r="W49" s="12"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="11"/>
     </row>
     <row r="50" spans="1:23" ht="15">
-      <c r="A50" s="16">
-        <f t="shared" ref="A50:A52" si="0">A49+1</f>
+      <c r="A50" s="15">
+        <f t="shared" ref="A50:A53" si="0">A49+1</f>
         <v>3</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18" t="s">
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="H50" s="18" t="s">
+      <c r="H50" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="I50" s="105" t="s">
+      <c r="I50" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="J50" s="18"/>
-      <c r="K50" s="87" t="s">
+      <c r="J50" s="17"/>
+      <c r="K50" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="L50" s="87" t="s">
+      <c r="L50" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="M50" s="87" t="s">
+      <c r="M50" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18" t="s">
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="T50" s="19"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="12"/>
+      <c r="T50" s="18"/>
+      <c r="U50" s="18"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="11"/>
     </row>
     <row r="51" spans="1:23" ht="30">
-      <c r="A51" s="16">
+      <c r="A51" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="105" t="s">
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="J51" s="18"/>
-      <c r="K51" s="87" t="s">
+      <c r="J51" s="17"/>
+      <c r="K51" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="L51" s="87"/>
-      <c r="M51" s="87" t="s">
+      <c r="L51" s="78"/>
+      <c r="M51" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18" t="s">
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="20"/>
-      <c r="W51" s="12"/>
+      <c r="T51" s="18"/>
+      <c r="U51" s="18"/>
+      <c r="V51" s="19"/>
+      <c r="W51" s="11"/>
     </row>
     <row r="52" spans="1:23">
-      <c r="A52" s="16">
+      <c r="A52" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="105"/>
-      <c r="J52" s="18" t="b">
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="K52" s="87"/>
-      <c r="L52" s="87"/>
-      <c r="M52" s="87"/>
-      <c r="N52" s="18"/>
-      <c r="O52" s="18"/>
-      <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18" t="s">
+      <c r="K52" s="78"/>
+      <c r="L52" s="78"/>
+      <c r="M52" s="78"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17"/>
+      <c r="S52" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="T52" s="19"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="20"/>
-      <c r="W52" s="12"/>
+      <c r="T52" s="18"/>
+      <c r="U52" s="18"/>
+      <c r="V52" s="19"/>
+      <c r="W52" s="11"/>
     </row>
     <row r="53" spans="1:23">
-      <c r="A53" s="16"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="87"/>
-      <c r="L53" s="87"/>
-      <c r="M53" s="87"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="20"/>
-      <c r="W53" s="12"/>
+      <c r="A53" s="15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="K53" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="L53" s="78"/>
+      <c r="M53" s="78"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="11"/>
     </row>
     <row r="54" spans="1:23">
-      <c r="A54" s="16"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="88"/>
-      <c r="L54" s="88"/>
-      <c r="M54" s="87"/>
-      <c r="N54" s="42"/>
-      <c r="O54" s="42"/>
-      <c r="P54" s="42"/>
-      <c r="Q54" s="42"/>
-      <c r="R54" s="42"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="19"/>
-      <c r="U54" s="19"/>
-      <c r="V54" s="20"/>
-      <c r="W54" s="12"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="78"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="40"/>
+      <c r="P54" s="40"/>
+      <c r="Q54" s="40"/>
+      <c r="R54" s="40"/>
+      <c r="S54" s="17"/>
+      <c r="T54" s="18"/>
+      <c r="U54" s="18"/>
+      <c r="V54" s="19"/>
+      <c r="W54" s="11"/>
     </row>
     <row r="55" spans="1:23">
-      <c r="A55" s="16"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="87"/>
-      <c r="L55" s="87"/>
-      <c r="M55" s="87"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="19"/>
-      <c r="U55" s="19"/>
-      <c r="V55" s="20"/>
-      <c r="W55" s="12"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="78"/>
+      <c r="L55" s="78"/>
+      <c r="M55" s="78"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="17"/>
+      <c r="T55" s="18"/>
+      <c r="U55" s="18"/>
+      <c r="V55" s="19"/>
+      <c r="W55" s="11"/>
     </row>
     <row r="56" spans="1:23">
-      <c r="A56" s="16"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="42"/>
-      <c r="J56" s="42"/>
-      <c r="K56" s="88"/>
-      <c r="L56" s="88"/>
-      <c r="M56" s="87"/>
-      <c r="N56" s="42"/>
-      <c r="O56" s="42"/>
-      <c r="P56" s="42"/>
-      <c r="Q56" s="42"/>
-      <c r="R56" s="42"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="19"/>
-      <c r="U56" s="19"/>
-      <c r="V56" s="20"/>
-      <c r="W56" s="12"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="79"/>
+      <c r="M56" s="78"/>
+      <c r="N56" s="40"/>
+      <c r="O56" s="40"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="40"/>
+      <c r="R56" s="40"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="18"/>
+      <c r="U56" s="18"/>
+      <c r="V56" s="19"/>
+      <c r="W56" s="11"/>
     </row>
     <row r="57" spans="1:23">
-      <c r="A57" s="16"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="87"/>
-      <c r="L57" s="87"/>
-      <c r="M57" s="87"/>
-      <c r="N57" s="18"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
-      <c r="S57" s="18"/>
-      <c r="T57" s="19"/>
-      <c r="U57" s="19"/>
-      <c r="V57" s="20"/>
-      <c r="W57" s="12"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="78"/>
+      <c r="L57" s="78"/>
+      <c r="M57" s="78"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="18"/>
+      <c r="U57" s="18"/>
+      <c r="V57" s="19"/>
+      <c r="W57" s="11"/>
     </row>
     <row r="58" spans="1:23">
-      <c r="A58" s="16"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="42"/>
-      <c r="J58" s="42"/>
-      <c r="K58" s="88"/>
-      <c r="L58" s="88"/>
-      <c r="M58" s="87"/>
-      <c r="N58" s="42"/>
-      <c r="O58" s="42"/>
-      <c r="P58" s="42"/>
-      <c r="Q58" s="42"/>
-      <c r="R58" s="42"/>
-      <c r="S58" s="18"/>
-      <c r="T58" s="19"/>
-      <c r="U58" s="19"/>
-      <c r="V58" s="20"/>
-      <c r="W58" s="12"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="78"/>
+      <c r="N58" s="40"/>
+      <c r="O58" s="40"/>
+      <c r="P58" s="40"/>
+      <c r="Q58" s="40"/>
+      <c r="R58" s="40"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="18"/>
+      <c r="U58" s="18"/>
+      <c r="V58" s="19"/>
+      <c r="W58" s="11"/>
     </row>
     <row r="59" spans="1:23">
-      <c r="A59" s="16"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="87"/>
-      <c r="L59" s="87"/>
-      <c r="M59" s="87"/>
-      <c r="N59" s="18"/>
-      <c r="O59" s="18"/>
-      <c r="P59" s="18"/>
-      <c r="Q59" s="18"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="18"/>
-      <c r="T59" s="19"/>
-      <c r="U59" s="19"/>
-      <c r="V59" s="20"/>
-      <c r="W59" s="12"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="78"/>
+      <c r="L59" s="78"/>
+      <c r="M59" s="78"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="18"/>
+      <c r="U59" s="18"/>
+      <c r="V59" s="19"/>
+      <c r="W59" s="11"/>
     </row>
     <row r="60" spans="1:23">
-      <c r="A60" s="16"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="87"/>
-      <c r="L60" s="87"/>
-      <c r="M60" s="87"/>
-      <c r="N60" s="18"/>
-      <c r="O60" s="18"/>
-      <c r="P60" s="18"/>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="18"/>
-      <c r="T60" s="19"/>
-      <c r="U60" s="19"/>
-      <c r="V60" s="20"/>
-      <c r="W60" s="12"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="78"/>
+      <c r="L60" s="78"/>
+      <c r="M60" s="78"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17"/>
+      <c r="R60" s="17"/>
+      <c r="S60" s="17"/>
+      <c r="T60" s="18"/>
+      <c r="U60" s="18"/>
+      <c r="V60" s="19"/>
+      <c r="W60" s="11"/>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" s="16"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="87"/>
-      <c r="L61" s="87"/>
-      <c r="M61" s="87"/>
-      <c r="N61" s="18"/>
-      <c r="O61" s="18"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="18"/>
-      <c r="T61" s="19"/>
-      <c r="U61" s="19"/>
-      <c r="V61" s="20"/>
-      <c r="W61" s="12"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="78"/>
+      <c r="L61" s="78"/>
+      <c r="M61" s="78"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17"/>
+      <c r="R61" s="17"/>
+      <c r="S61" s="17"/>
+      <c r="T61" s="18"/>
+      <c r="U61" s="18"/>
+      <c r="V61" s="19"/>
+      <c r="W61" s="11"/>
     </row>
     <row r="62" spans="1:23">
-      <c r="A62" s="16"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="87"/>
-      <c r="L62" s="87"/>
-      <c r="M62" s="87"/>
-      <c r="N62" s="18"/>
-      <c r="O62" s="18"/>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="18"/>
-      <c r="S62" s="18"/>
-      <c r="T62" s="19"/>
-      <c r="U62" s="19"/>
-      <c r="V62" s="20"/>
-      <c r="W62" s="12"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="78"/>
+      <c r="L62" s="78"/>
+      <c r="M62" s="78"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17"/>
+      <c r="R62" s="17"/>
+      <c r="S62" s="17"/>
+      <c r="T62" s="18"/>
+      <c r="U62" s="18"/>
+      <c r="V62" s="19"/>
+      <c r="W62" s="11"/>
     </row>
     <row r="63" spans="1:23">
-      <c r="A63" s="16"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="87"/>
-      <c r="L63" s="87"/>
-      <c r="M63" s="87"/>
-      <c r="N63" s="18"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="18"/>
-      <c r="S63" s="18"/>
-      <c r="T63" s="19"/>
-      <c r="U63" s="19"/>
-      <c r="V63" s="20"/>
-      <c r="W63" s="12"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="78"/>
+      <c r="L63" s="78"/>
+      <c r="M63" s="78"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="17"/>
+      <c r="S63" s="17"/>
+      <c r="T63" s="18"/>
+      <c r="U63" s="18"/>
+      <c r="V63" s="19"/>
+      <c r="W63" s="11"/>
     </row>
     <row r="64" spans="1:23">
-      <c r="A64" s="21"/>
-      <c r="B64" s="22"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="89"/>
-      <c r="L64" s="89"/>
-      <c r="M64" s="96"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="23"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="23"/>
-      <c r="S64" s="23"/>
-      <c r="T64" s="24"/>
-      <c r="U64" s="24"/>
-      <c r="V64" s="25"/>
-      <c r="W64" s="12"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="80"/>
+      <c r="L64" s="80"/>
+      <c r="M64" s="87"/>
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
+      <c r="P64" s="22"/>
+      <c r="Q64" s="22"/>
+      <c r="R64" s="22"/>
+      <c r="S64" s="22"/>
+      <c r="T64" s="23"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="24"/>
+      <c r="W64" s="11"/>
     </row>
     <row r="75" spans="11:11">
-      <c r="K75" s="31">
+      <c r="K75" s="1">
         <v>9</v>
       </c>
     </row>
@@ -3854,107 +3638,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="45" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="45" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="45" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="45" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="45" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="45" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="15" max="261" width="8.83203125" style="45" customWidth="1"/>
-    <col min="262" max="16384" width="10.83203125" style="45"/>
+    <col min="1" max="3" width="8.83203125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="43" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="43" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="43" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="43" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="15" max="261" width="8.83203125" style="43" customWidth="1"/>
+    <col min="262" max="16384" width="10.83203125" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="19">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="44"/>
+      <c r="R1" s="42"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="75" t="s">
+      <c r="J3" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="75" t="s">
+      <c r="L3" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="75" t="s">
+      <c r="N3" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="75" t="s">
+      <c r="P3" s="73" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="B4" s="91"/>
-      <c r="D4" s="92" t="s">
+      <c r="B4" s="82"/>
+      <c r="D4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="P4" s="46"/>
+      <c r="H4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="P4" s="44"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="93"/>
-      <c r="F5" s="48"/>
-      <c r="H5" s="48" t="s">
+      <c r="D5" s="84"/>
+      <c r="F5" s="46"/>
+      <c r="H5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="48" t="s">
+      <c r="L5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="48" t="s">
+      <c r="N5" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="48" t="s">
+      <c r="P5" s="46" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="B6" s="94"/>
+      <c r="B6" s="85"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>